<commit_message>
add fr core 2.1.0
</commit_message>
<xml_diff>
--- a/www/ig/fhir/core/CodeSystem-fr-core-cs-circonstances-sortie.xlsx
+++ b/www/ig/fhir/core/CodeSystem-fr-core-cs-circonstances-sortie.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.1</t>
+    <t>2.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-16T11:49:14+02:00</t>
+    <t>2024-09-04T10:06:33+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -75,7 +75,7 @@
     <t>Interop'Santé (http://interopsante.org/)</t>
   </si>
   <si>
-    <t>InteropSanté (fhir@interopsante.org(WORK))</t>
+    <t>InteropSanté (fhir@interopsante.org(work))</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>